<commit_message>
Second update after a week
</commit_message>
<xml_diff>
--- a/Microprocessor/LAB 5/DELAY TIME.xlsx
+++ b/Microprocessor/LAB 5/DELAY TIME.xlsx
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>